<commit_message>
Refactor discrepancy report; LST heats shouldn't be continuous
</commit_message>
<xml_diff>
--- a/schedule2013.xlsx
+++ b/schedule2013.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3840" uniqueCount="1019">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3839" uniqueCount="1019">
   <si>
     <t>Date</t>
   </si>
@@ -3200,26 +3200,26 @@
   </sheetPr>
   <dimension ref="A1:L740"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A361" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H378" activeCellId="0" pane="topLeft" sqref="H378"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.79607843137255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.49411764705882"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.43137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.94901960784314"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.72156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5843137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.1450980392157"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4627450980392"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.5372549019608"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.8"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="1.44313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.83921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.51372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.46274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.97647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2509803921569"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.6627450980392"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.2156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5137254901961"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.7176470588235"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.8509803921569"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="1.44705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.63921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1" s="2">
@@ -14327,9 +14327,6 @@
       </c>
       <c r="G378" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="H378" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="I378" s="1" t="s">
         <v>566</v>

</xml_diff>